<commit_message>
feat: Update Issue 5 (Product)
</commit_message>
<xml_diff>
--- a/public/template/report/Template_Report_Product_Reminders.xlsx
+++ b/public/template/report/Template_Report_Product_Reminders.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\Kerjaan\Project\rpc-be\public\template\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF40CBD3-007D-46A5-9FF0-188262911F7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74F65AB1-5A8C-481C-9420-A6B1AF147F65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0674CD87-AF00-EC40-A640-CA30B1852CB8}"/>
   </bookViews>
   <sheets>
-    <sheet name="Report Growth" sheetId="1" r:id="rId1"/>
+    <sheet name="Report Product Reminders" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>

</xml_diff>